<commit_message>
Project plan and gantt chart updated
</commit_message>
<xml_diff>
--- a/Gantt chart.xlsx
+++ b/Gantt chart.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/797c1e1ebe0f8e78/Pictures/softwaretech/2810ICT-7810ICT-2023-Assignment/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="11_E0C8A7F0515C29AAE5B1393562E56DCE2A14542E" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="146" documentId="11_E0C8A7F0515C29AAE5B1393562E56DCE2A14542E" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{7F5B2AFB-E943-4E31-A23B-4B9C8D405DD6}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -366,7 +366,7 @@
       <scheme val="major"/>
     </font>
   </fonts>
-  <fills count="8">
+  <fills count="9">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -405,6 +405,12 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="9"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFF00"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -552,7 +558,7 @@
       <alignment horizontal="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="37">
+  <cellXfs count="38">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -625,6 +631,36 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="5" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="5" xfId="10" applyBorder="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="2" xfId="10" applyBorder="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="6" xfId="5" applyFont="1" applyBorder="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="5" applyFont="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="7" xfId="5" applyFont="1" applyBorder="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="5" applyFont="1" applyBorder="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="5" applyFont="1" applyBorder="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="5" applyFont="1" applyBorder="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="5" applyFont="1" applyBorder="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="12">
       <alignment vertical="center"/>
     </xf>
@@ -636,33 +672,6 @@
     </xf>
     <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="10">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="2" xfId="10" applyBorder="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="5" xfId="10" applyBorder="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="6" xfId="5" applyFont="1" applyBorder="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="5" applyFont="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="7" xfId="5" applyFont="1" applyBorder="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="5" applyFont="1" applyBorder="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="5" applyFont="1" applyBorder="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="5" applyFont="1" applyBorder="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="5" applyFont="1" applyBorder="1">
-      <alignment horizontal="left" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="19">
@@ -686,7 +695,120 @@
     <cellStyle name="Project Headers" xfId="4" xr:uid="{00000000-0005-0000-0000-000011000000}"/>
     <cellStyle name="Title" xfId="8" builtinId="15" customBuiltin="1"/>
   </cellStyles>
-  <dxfs count="9">
+  <dxfs count="17">
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="0"/>
+        </patternFill>
+      </fill>
+      <border>
+        <bottom style="thin">
+          <color theme="0"/>
+        </bottom>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="0" tint="-4.9989318521683403E-2"/>
+        </patternFill>
+      </fill>
+      <border>
+        <bottom style="thin">
+          <color theme="0"/>
+        </bottom>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="9" tint="0.59996337778862885"/>
+        </patternFill>
+      </fill>
+      <border>
+        <left style="thin">
+          <color theme="9" tint="-0.24994659260841701"/>
+        </left>
+        <right style="thin">
+          <color theme="9" tint="-0.24994659260841701"/>
+        </right>
+        <bottom style="thin">
+          <color theme="9" tint="0.59996337778862885"/>
+        </bottom>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="lightUp">
+          <fgColor theme="7"/>
+          <bgColor auto="1"/>
+        </patternFill>
+      </fill>
+      <border>
+        <bottom style="thin">
+          <color theme="0"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="lightUp">
+          <fgColor theme="7"/>
+          <bgColor theme="9" tint="0.59996337778862885"/>
+        </patternFill>
+      </fill>
+      <border>
+        <bottom style="thin">
+          <color theme="0"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="lightUp">
+          <fgColor theme="7"/>
+          <bgColor theme="7" tint="0.59996337778862885"/>
+        </patternFill>
+      </fill>
+      <border>
+        <bottom style="thin">
+          <color theme="0"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor auto="1"/>
+          <bgColor theme="9"/>
+        </patternFill>
+      </fill>
+      <border>
+        <bottom style="thin">
+          <color theme="0"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor auto="1"/>
+          <bgColor theme="7"/>
+        </patternFill>
+      </fill>
+      <border>
+        <bottom style="thin">
+          <color theme="0"/>
+        </bottom>
+      </border>
+    </dxf>
     <dxf>
       <fill>
         <patternFill>
@@ -831,6 +953,10 @@
     </ext>
   </extLst>
 </styleSheet>
+</file>
+
+<file path=xl/persons/person.xml><?xml version="1.0" encoding="utf-8"?>
+<personList xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main"/>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -1066,21 +1192,24 @@
   </sheetPr>
   <dimension ref="B1:BO39"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" topLeftCell="D1" zoomScaleNormal="100" zoomScaleSheetLayoutView="80" workbookViewId="0">
-      <selection activeCell="M6" sqref="M6"/>
+    <sheetView showGridLines="0" tabSelected="1" zoomScale="34" zoomScaleNormal="100" zoomScaleSheetLayoutView="80" workbookViewId="0">
+      <selection activeCell="DD1" sqref="DD1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="2.77734375" defaultRowHeight="30" customHeight="1" x14ac:dyDescent="0.35"/>
   <cols>
     <col min="1" max="1" width="2.6640625" customWidth="1"/>
     <col min="2" max="2" width="26.33203125" style="2" customWidth="1"/>
-    <col min="3" max="3" width="11.33203125" style="1" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="10.109375" style="1" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="7.77734375" style="1" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="10.109375" style="1" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="15.44140625" style="4" bestFit="1" customWidth="1"/>
-    <col min="8" max="27" width="2.77734375" style="1"/>
+    <col min="3" max="3" width="11.44140625" style="1" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="10.21875" style="1" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="7.88671875" style="1" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="10.21875" style="1" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="15.5546875" style="4" bestFit="1" customWidth="1"/>
+    <col min="8" max="16" width="3.88671875" style="1" bestFit="1" customWidth="1"/>
+    <col min="17" max="27" width="5.44140625" style="1" bestFit="1" customWidth="1"/>
+    <col min="28" max="41" width="5.44140625" bestFit="1" customWidth="1"/>
     <col min="42" max="42" width="2.77734375" customWidth="1"/>
+    <col min="43" max="67" width="5.44140625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="2:67" ht="60" customHeight="1" thickBot="1" x14ac:dyDescent="1.05">
@@ -1094,13 +1223,13 @@
       <c r="G1" s="13"/>
     </row>
     <row r="2" spans="2:67" ht="21" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B2" s="24" t="s">
+      <c r="B2" s="34" t="s">
         <v>39</v>
       </c>
-      <c r="C2" s="24"/>
-      <c r="D2" s="24"/>
-      <c r="E2" s="24"/>
-      <c r="F2" s="24"/>
+      <c r="C2" s="34"/>
+      <c r="D2" s="34"/>
+      <c r="E2" s="34"/>
+      <c r="F2" s="34"/>
       <c r="G2" s="5" t="s">
         <v>31</v>
       </c>
@@ -1108,37 +1237,37 @@
         <v>1</v>
       </c>
       <c r="J2" s="16"/>
-      <c r="K2" s="30" t="s">
+      <c r="K2" s="27" t="s">
         <v>38</v>
       </c>
-      <c r="L2" s="31"/>
-      <c r="M2" s="31"/>
-      <c r="N2" s="31"/>
-      <c r="O2" s="32"/>
+      <c r="L2" s="28"/>
+      <c r="M2" s="28"/>
+      <c r="N2" s="28"/>
+      <c r="O2" s="29"/>
       <c r="P2" s="17"/>
-      <c r="Q2" s="30" t="s">
+      <c r="Q2" s="27" t="s">
         <v>37</v>
       </c>
-      <c r="R2" s="33"/>
-      <c r="S2" s="33"/>
-      <c r="T2" s="32"/>
+      <c r="R2" s="30"/>
+      <c r="S2" s="30"/>
+      <c r="T2" s="29"/>
       <c r="U2" s="18"/>
-      <c r="V2" s="34" t="s">
+      <c r="V2" s="31" t="s">
         <v>28</v>
       </c>
-      <c r="W2" s="35"/>
-      <c r="X2" s="35"/>
-      <c r="Y2" s="36"/>
+      <c r="W2" s="32"/>
+      <c r="X2" s="32"/>
+      <c r="Y2" s="33"/>
       <c r="Z2" s="19"/>
-      <c r="AA2" s="34" t="s">
+      <c r="AA2" s="31" t="s">
         <v>29</v>
       </c>
-      <c r="AB2" s="35"/>
-      <c r="AC2" s="35"/>
-      <c r="AD2" s="35"/>
-      <c r="AE2" s="35"/>
-      <c r="AF2" s="35"/>
-      <c r="AG2" s="36"/>
+      <c r="AB2" s="32"/>
+      <c r="AC2" s="32"/>
+      <c r="AD2" s="32"/>
+      <c r="AE2" s="32"/>
+      <c r="AF2" s="32"/>
+      <c r="AG2" s="33"/>
       <c r="AH2" s="20"/>
       <c r="AI2" s="22" t="s">
         <v>30</v>
@@ -1152,22 +1281,22 @@
       <c r="AP2" s="23"/>
     </row>
     <row r="3" spans="2:67" s="12" customFormat="1" ht="39.9" customHeight="1" thickTop="1" x14ac:dyDescent="0.3">
-      <c r="B3" s="25" t="s">
-        <v>1</v>
-      </c>
-      <c r="C3" s="27" t="s">
+      <c r="B3" s="35" t="s">
+        <v>1</v>
+      </c>
+      <c r="C3" s="37" t="s">
         <v>32</v>
       </c>
-      <c r="D3" s="27" t="s">
+      <c r="D3" s="37" t="s">
         <v>33</v>
       </c>
-      <c r="E3" s="27" t="s">
+      <c r="E3" s="37" t="s">
         <v>34</v>
       </c>
-      <c r="F3" s="27" t="s">
+      <c r="F3" s="37" t="s">
         <v>35</v>
       </c>
-      <c r="G3" s="29" t="s">
+      <c r="G3" s="25" t="s">
         <v>36</v>
       </c>
       <c r="H3" s="21" t="s">
@@ -1193,13 +1322,13 @@
       <c r="Z3" s="11"/>
       <c r="AA3" s="11"/>
     </row>
-    <row r="4" spans="2:67" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B4" s="26"/>
-      <c r="C4" s="28"/>
-      <c r="D4" s="28"/>
-      <c r="E4" s="28"/>
-      <c r="F4" s="28"/>
-      <c r="G4" s="28"/>
+    <row r="4" spans="2:67" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="B4" s="36"/>
+      <c r="C4" s="26"/>
+      <c r="D4" s="26"/>
+      <c r="E4" s="26"/>
+      <c r="F4" s="26"/>
+      <c r="G4" s="26"/>
       <c r="H4" s="3">
         <v>1</v>
       </c>
@@ -1381,7 +1510,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="5" spans="2:67" ht="30" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="5" spans="2:67" ht="30" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.4">
       <c r="B5" s="6" t="s">
         <v>2</v>
       </c>
@@ -1389,188 +1518,315 @@
         <v>1</v>
       </c>
       <c r="D5" s="7">
-        <v>5</v>
-      </c>
-      <c r="E5" s="7"/>
-      <c r="F5" s="7"/>
+        <v>1</v>
+      </c>
+      <c r="E5" s="7">
+        <v>1</v>
+      </c>
+      <c r="F5" s="7">
+        <v>1</v>
+      </c>
       <c r="G5" s="8">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="6" spans="2:67" ht="30" customHeight="1" x14ac:dyDescent="0.35">
+        <v>1</v>
+      </c>
+      <c r="H5" s="18"/>
+      <c r="I5" s="24"/>
+      <c r="J5" s="24"/>
+      <c r="K5" s="24"/>
+      <c r="L5" s="24"/>
+    </row>
+    <row r="6" spans="2:67" ht="30" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.4">
       <c r="B6" s="6" t="s">
         <v>3</v>
       </c>
-      <c r="C6" s="7"/>
-      <c r="D6" s="7"/>
-      <c r="E6" s="7"/>
-      <c r="F6" s="7"/>
+      <c r="C6" s="7">
+        <v>1</v>
+      </c>
+      <c r="D6" s="7">
+        <v>1</v>
+      </c>
+      <c r="E6" s="7">
+        <v>1</v>
+      </c>
+      <c r="F6" s="7">
+        <v>1</v>
+      </c>
       <c r="G6" s="8">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="7" spans="2:67" ht="30" customHeight="1" x14ac:dyDescent="0.35">
+        <v>1</v>
+      </c>
+      <c r="H6" s="18"/>
+      <c r="L6" s="17"/>
+    </row>
+    <row r="7" spans="2:67" ht="30" customHeight="1" thickTop="1" x14ac:dyDescent="0.35">
       <c r="B7" s="6" t="s">
         <v>4</v>
       </c>
-      <c r="C7" s="7"/>
-      <c r="D7" s="7"/>
-      <c r="E7" s="7"/>
-      <c r="F7" s="7"/>
+      <c r="C7" s="7">
+        <v>2</v>
+      </c>
+      <c r="D7" s="7">
+        <v>2</v>
+      </c>
+      <c r="E7" s="7">
+        <v>2</v>
+      </c>
+      <c r="F7" s="7">
+        <v>2</v>
+      </c>
       <c r="G7" s="8">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="8" spans="2:67" ht="30" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B8" s="6" t="s">
         <v>5</v>
       </c>
-      <c r="C8" s="7"/>
-      <c r="D8" s="7"/>
-      <c r="E8" s="7"/>
-      <c r="F8" s="7"/>
+      <c r="C8" s="7">
+        <v>2</v>
+      </c>
+      <c r="D8" s="7">
+        <v>2</v>
+      </c>
+      <c r="E8" s="7">
+        <v>2</v>
+      </c>
+      <c r="F8" s="7">
+        <v>2</v>
+      </c>
       <c r="G8" s="8">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="9" spans="2:67" ht="30" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B9" s="6" t="s">
         <v>6</v>
       </c>
-      <c r="C9" s="7"/>
-      <c r="D9" s="7"/>
-      <c r="E9" s="7"/>
-      <c r="F9" s="7"/>
+      <c r="C9" s="7">
+        <v>2</v>
+      </c>
+      <c r="D9" s="7">
+        <v>2</v>
+      </c>
+      <c r="E9" s="7">
+        <v>2</v>
+      </c>
+      <c r="F9" s="7">
+        <v>2</v>
+      </c>
       <c r="G9" s="8">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="10" spans="2:67" ht="30" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B10" s="6" t="s">
         <v>7</v>
       </c>
-      <c r="C10" s="7"/>
-      <c r="D10" s="7"/>
-      <c r="E10" s="7"/>
-      <c r="F10" s="7"/>
+      <c r="C10" s="7">
+        <v>3</v>
+      </c>
+      <c r="D10" s="7">
+        <v>3</v>
+      </c>
+      <c r="E10" s="7">
+        <v>3</v>
+      </c>
+      <c r="F10" s="7">
+        <v>3</v>
+      </c>
       <c r="G10" s="8">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="11" spans="2:67" ht="30" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B11" s="6" t="s">
         <v>8</v>
       </c>
-      <c r="C11" s="7"/>
-      <c r="D11" s="7"/>
-      <c r="E11" s="7"/>
-      <c r="F11" s="7"/>
+      <c r="C11" s="7">
+        <v>3</v>
+      </c>
+      <c r="D11" s="7">
+        <v>3</v>
+      </c>
+      <c r="E11" s="7">
+        <v>3</v>
+      </c>
+      <c r="F11" s="7">
+        <v>3</v>
+      </c>
       <c r="G11" s="8">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="12" spans="2:67" ht="30" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B12" s="6" t="s">
         <v>9</v>
       </c>
-      <c r="C12" s="7"/>
-      <c r="D12" s="7"/>
-      <c r="E12" s="7"/>
-      <c r="F12" s="7"/>
+      <c r="C12" s="7">
+        <v>3</v>
+      </c>
+      <c r="D12" s="7">
+        <v>3</v>
+      </c>
+      <c r="E12" s="7">
+        <v>3</v>
+      </c>
+      <c r="F12" s="7">
+        <v>3</v>
+      </c>
       <c r="G12" s="8">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="13" spans="2:67" ht="30" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B13" s="6" t="s">
         <v>10</v>
       </c>
-      <c r="C13" s="7"/>
-      <c r="D13" s="7"/>
-      <c r="E13" s="7"/>
-      <c r="F13" s="7"/>
+      <c r="C13" s="7">
+        <v>4</v>
+      </c>
+      <c r="D13" s="7">
+        <v>4</v>
+      </c>
+      <c r="E13" s="7">
+        <v>4</v>
+      </c>
+      <c r="F13" s="7">
+        <v>4</v>
+      </c>
       <c r="G13" s="8">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="14" spans="2:67" ht="30" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B14" s="6" t="s">
         <v>11</v>
       </c>
-      <c r="C14" s="7"/>
-      <c r="D14" s="7"/>
-      <c r="E14" s="7"/>
-      <c r="F14" s="7"/>
+      <c r="C14" s="7">
+        <v>4</v>
+      </c>
+      <c r="D14" s="7">
+        <v>4</v>
+      </c>
+      <c r="E14" s="7">
+        <v>4</v>
+      </c>
+      <c r="F14" s="7">
+        <v>4</v>
+      </c>
       <c r="G14" s="8">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="15" spans="2:67" ht="30" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B15" s="6" t="s">
         <v>12</v>
       </c>
-      <c r="C15" s="9"/>
-      <c r="D15" s="7"/>
-      <c r="E15" s="7"/>
-      <c r="F15" s="7"/>
+      <c r="C15" s="9">
+        <v>4</v>
+      </c>
+      <c r="D15" s="7">
+        <v>4</v>
+      </c>
+      <c r="E15" s="7">
+        <v>4</v>
+      </c>
+      <c r="F15" s="7">
+        <v>4</v>
+      </c>
       <c r="G15" s="8">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="16" spans="2:67" ht="30" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B16" s="6" t="s">
         <v>13</v>
       </c>
-      <c r="C16" s="7"/>
-      <c r="D16" s="7"/>
-      <c r="E16" s="7"/>
-      <c r="F16" s="7"/>
+      <c r="C16" s="7">
+        <v>5</v>
+      </c>
+      <c r="D16" s="7">
+        <v>5</v>
+      </c>
+      <c r="E16" s="7">
+        <v>5</v>
+      </c>
+      <c r="F16" s="7">
+        <v>5</v>
+      </c>
       <c r="G16" s="8">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="17" spans="2:7" ht="30" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B17" s="6" t="s">
         <v>14</v>
       </c>
-      <c r="C17" s="7"/>
-      <c r="D17" s="7"/>
-      <c r="E17" s="7"/>
-      <c r="F17" s="7"/>
+      <c r="C17" s="7">
+        <v>5</v>
+      </c>
+      <c r="D17" s="7">
+        <v>5</v>
+      </c>
+      <c r="E17" s="7">
+        <v>5</v>
+      </c>
+      <c r="F17" s="7">
+        <v>5</v>
+      </c>
       <c r="G17" s="8">
-        <v>0</v>
+        <v>0.9</v>
       </c>
     </row>
     <row r="18" spans="2:7" ht="30" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B18" s="6" t="s">
         <v>15</v>
       </c>
-      <c r="C18" s="7"/>
-      <c r="D18" s="7"/>
-      <c r="E18" s="7"/>
-      <c r="F18" s="7"/>
+      <c r="C18" s="7">
+        <v>6</v>
+      </c>
+      <c r="D18" s="7">
+        <v>6</v>
+      </c>
+      <c r="E18" s="7">
+        <v>6</v>
+      </c>
+      <c r="F18" s="7">
+        <v>6</v>
+      </c>
       <c r="G18" s="8">
-        <v>0</v>
+        <v>0.9</v>
       </c>
     </row>
     <row r="19" spans="2:7" ht="30" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B19" s="6" t="s">
         <v>16</v>
       </c>
-      <c r="C19" s="7"/>
-      <c r="D19" s="7"/>
-      <c r="E19" s="7"/>
-      <c r="F19" s="7"/>
+      <c r="C19" s="7">
+        <v>6</v>
+      </c>
+      <c r="D19" s="7">
+        <v>6</v>
+      </c>
+      <c r="E19" s="7">
+        <v>6</v>
+      </c>
+      <c r="F19" s="7">
+        <v>6</v>
+      </c>
       <c r="G19" s="8">
-        <v>0</v>
+        <v>0.5</v>
       </c>
     </row>
     <row r="20" spans="2:7" ht="30" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B20" s="6" t="s">
         <v>17</v>
       </c>
-      <c r="C20" s="7"/>
-      <c r="D20" s="7"/>
+      <c r="C20" s="7">
+        <v>7</v>
+      </c>
+      <c r="D20" s="7">
+        <v>8</v>
+      </c>
       <c r="E20" s="7"/>
       <c r="F20" s="7"/>
       <c r="G20" s="8">
@@ -1581,8 +1837,12 @@
       <c r="B21" s="6" t="s">
         <v>18</v>
       </c>
-      <c r="C21" s="7"/>
-      <c r="D21" s="7"/>
+      <c r="C21" s="7">
+        <v>9</v>
+      </c>
+      <c r="D21" s="7">
+        <v>14</v>
+      </c>
       <c r="E21" s="7"/>
       <c r="F21" s="7"/>
       <c r="G21" s="8">
@@ -1593,8 +1853,12 @@
       <c r="B22" s="6" t="s">
         <v>19</v>
       </c>
-      <c r="C22" s="7"/>
-      <c r="D22" s="7"/>
+      <c r="C22" s="7">
+        <v>15</v>
+      </c>
+      <c r="D22" s="7">
+        <v>15</v>
+      </c>
       <c r="E22" s="7"/>
       <c r="F22" s="7"/>
       <c r="G22" s="8">
@@ -1605,8 +1869,12 @@
       <c r="B23" s="6" t="s">
         <v>20</v>
       </c>
-      <c r="C23" s="7"/>
-      <c r="D23" s="7"/>
+      <c r="C23" s="7">
+        <v>16</v>
+      </c>
+      <c r="D23" s="7">
+        <v>16</v>
+      </c>
       <c r="E23" s="7"/>
       <c r="F23" s="7"/>
       <c r="G23" s="8">
@@ -1617,8 +1885,12 @@
       <c r="B24" s="6" t="s">
         <v>21</v>
       </c>
-      <c r="C24" s="7"/>
-      <c r="D24" s="7"/>
+      <c r="C24" s="7">
+        <v>17</v>
+      </c>
+      <c r="D24" s="7">
+        <v>17</v>
+      </c>
       <c r="E24" s="7"/>
       <c r="F24" s="7"/>
       <c r="G24" s="8">
@@ -1629,8 +1901,12 @@
       <c r="B25" s="6" t="s">
         <v>22</v>
       </c>
-      <c r="C25" s="7"/>
-      <c r="D25" s="7"/>
+      <c r="C25" s="7">
+        <v>17</v>
+      </c>
+      <c r="D25" s="7">
+        <v>17</v>
+      </c>
       <c r="E25" s="7"/>
       <c r="F25" s="7"/>
       <c r="G25" s="8">
@@ -1641,8 +1917,12 @@
       <c r="B26" s="6" t="s">
         <v>23</v>
       </c>
-      <c r="C26" s="7"/>
-      <c r="D26" s="7"/>
+      <c r="C26" s="7">
+        <v>18</v>
+      </c>
+      <c r="D26" s="7">
+        <v>18</v>
+      </c>
       <c r="E26" s="7"/>
       <c r="F26" s="7"/>
       <c r="G26" s="8">
@@ -1653,8 +1933,12 @@
       <c r="B27" s="6" t="s">
         <v>24</v>
       </c>
-      <c r="C27" s="7"/>
-      <c r="D27" s="7"/>
+      <c r="C27" s="7">
+        <v>18</v>
+      </c>
+      <c r="D27" s="7">
+        <v>19</v>
+      </c>
       <c r="E27" s="7"/>
       <c r="F27" s="7"/>
       <c r="G27" s="8">
@@ -1665,8 +1949,12 @@
       <c r="B28" s="6" t="s">
         <v>25</v>
       </c>
-      <c r="C28" s="7"/>
-      <c r="D28" s="7"/>
+      <c r="C28" s="7">
+        <v>19</v>
+      </c>
+      <c r="D28" s="7">
+        <v>20</v>
+      </c>
       <c r="E28" s="7"/>
       <c r="F28" s="7"/>
       <c r="G28" s="8">
@@ -1677,8 +1965,12 @@
       <c r="B29" s="6" t="s">
         <v>26</v>
       </c>
-      <c r="C29" s="7"/>
-      <c r="D29" s="7"/>
+      <c r="C29" s="7">
+        <v>20</v>
+      </c>
+      <c r="D29" s="7">
+        <v>20</v>
+      </c>
       <c r="E29" s="7"/>
       <c r="F29" s="7"/>
       <c r="G29" s="8">
@@ -1689,8 +1981,12 @@
       <c r="B30" s="6" t="s">
         <v>27</v>
       </c>
-      <c r="C30" s="7"/>
-      <c r="D30" s="7"/>
+      <c r="C30" s="7">
+        <v>21</v>
+      </c>
+      <c r="D30" s="7">
+        <v>21</v>
+      </c>
       <c r="E30" s="7"/>
       <c r="F30" s="7"/>
       <c r="G30" s="8">
@@ -1701,8 +1997,12 @@
       <c r="B31" s="6" t="s">
         <v>40</v>
       </c>
-      <c r="C31" s="7"/>
-      <c r="D31" s="7"/>
+      <c r="C31" s="7">
+        <v>21</v>
+      </c>
+      <c r="D31" s="7">
+        <v>21</v>
+      </c>
       <c r="E31" s="7"/>
       <c r="F31" s="7"/>
       <c r="G31" s="8">
@@ -1713,8 +2013,12 @@
       <c r="B32" s="6" t="s">
         <v>41</v>
       </c>
-      <c r="C32" s="7"/>
-      <c r="D32" s="7"/>
+      <c r="C32" s="7">
+        <v>22</v>
+      </c>
+      <c r="D32" s="7">
+        <v>23</v>
+      </c>
       <c r="E32" s="7"/>
       <c r="F32" s="7"/>
       <c r="G32" s="8">
@@ -1725,8 +2029,12 @@
       <c r="B33" s="6" t="s">
         <v>42</v>
       </c>
-      <c r="C33" s="7"/>
-      <c r="D33" s="7"/>
+      <c r="C33" s="7">
+        <v>24</v>
+      </c>
+      <c r="D33" s="7">
+        <v>24</v>
+      </c>
       <c r="E33" s="7"/>
       <c r="F33" s="7"/>
       <c r="G33" s="8">
@@ -1807,46 +2115,46 @@
     </row>
   </sheetData>
   <mergeCells count="11">
-    <mergeCell ref="G3:G4"/>
-    <mergeCell ref="K2:O2"/>
-    <mergeCell ref="Q2:T2"/>
-    <mergeCell ref="V2:Y2"/>
-    <mergeCell ref="AA2:AG2"/>
     <mergeCell ref="B2:F2"/>
     <mergeCell ref="B3:B4"/>
     <mergeCell ref="C3:C4"/>
     <mergeCell ref="D3:D4"/>
     <mergeCell ref="E3:E4"/>
     <mergeCell ref="F3:F4"/>
+    <mergeCell ref="G3:G4"/>
+    <mergeCell ref="K2:O2"/>
+    <mergeCell ref="Q2:T2"/>
+    <mergeCell ref="V2:Y2"/>
+    <mergeCell ref="AA2:AG2"/>
   </mergeCells>
   <conditionalFormatting sqref="H4:BO4">
-    <cfRule type="expression" dxfId="8" priority="8">
+    <cfRule type="expression" dxfId="16" priority="8">
       <formula>H$4=period_selected</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="H5:BO39">
-    <cfRule type="expression" dxfId="7" priority="1">
+  <conditionalFormatting sqref="I5:BO5 I6:K6 M6:BO6 H7:BO39">
+    <cfRule type="expression" dxfId="15" priority="1">
       <formula>PercentComplete</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="6" priority="3">
+    <cfRule type="expression" dxfId="14" priority="3">
       <formula>PercentCompleteBeyond</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="5" priority="4">
+    <cfRule type="expression" dxfId="13" priority="4">
       <formula>Actual</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="4" priority="5">
+    <cfRule type="expression" dxfId="12" priority="5">
       <formula>ActualBeyond</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="3" priority="6">
+    <cfRule type="expression" dxfId="11" priority="6">
       <formula>Plan</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="2" priority="7">
+    <cfRule type="expression" dxfId="10" priority="7">
       <formula>H$4=period_selected</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="1" priority="11">
+    <cfRule type="expression" dxfId="9" priority="11">
       <formula>MOD(COLUMN(),2)</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="0" priority="12">
+    <cfRule type="expression" dxfId="8" priority="12">
       <formula>MOD(COLUMN(),2)=0</formula>
     </cfRule>
   </conditionalFormatting>

</xml_diff>

<commit_message>
Project Plan and Gantt Chart Update
</commit_message>
<xml_diff>
--- a/Gantt chart.xlsx
+++ b/Gantt chart.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="26731"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="10917"/>
   <workbookPr autoCompressPictures="0"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/797c1e1ebe0f8e78/Pictures/softwaretech/2810ICT-7810ICT-2023-Assignment/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/kartik/University/SoftwareTechnology/2810ICT-7810ICT-2023-Assignment/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="146" documentId="11_E0C8A7F0515C29AAE5B1393562E56DCE2A14542E" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{7F5B2AFB-E943-4E31-A23B-4B9C8D405DD6}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7B722E94-AD06-1242-BDD8-83D963BE3EA3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="36000" yWindow="0" windowWidth="38400" windowHeight="21600" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Project Planner" sheetId="1" r:id="rId1"/>
@@ -265,7 +265,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="14" x14ac:knownFonts="1">
+  <fonts count="15" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1" tint="0.24994659260841701"/>
@@ -364,6 +364,13 @@
       <name val="Corbel"/>
       <family val="2"/>
       <scheme val="major"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="13"/>
+      <color theme="7"/>
+      <name val="Calibri"/>
+      <family val="2"/>
     </font>
   </fonts>
   <fills count="9">
@@ -558,7 +565,7 @@
       <alignment horizontal="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="38">
+  <cellXfs count="39">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -634,12 +641,24 @@
     <xf numFmtId="0" fontId="0" fillId="8" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="12">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="9">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="2" xfId="9" applyBorder="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="10">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="2" xfId="10" applyBorder="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="10" fillId="0" borderId="5" xfId="10" applyBorder="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="2" xfId="10" applyBorder="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="6" xfId="5" applyFont="1" applyBorder="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
@@ -661,17 +680,8 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="5" applyFont="1" applyBorder="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="12">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="9">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="2" xfId="9" applyBorder="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="10">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    <xf numFmtId="9" fontId="14" fillId="0" borderId="0" xfId="6" applyFont="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="19">
@@ -695,7 +705,7 @@
     <cellStyle name="Project Headers" xfId="4" xr:uid="{00000000-0005-0000-0000-000011000000}"/>
     <cellStyle name="Title" xfId="8" builtinId="15" customBuiltin="1"/>
   </cellStyles>
-  <dxfs count="17">
+  <dxfs count="9">
     <dxf>
       <fill>
         <patternFill>
@@ -722,6 +732,19 @@
         </bottom>
         <vertical/>
         <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor auto="1"/>
+          <bgColor theme="7"/>
+        </patternFill>
+      </fill>
+      <border>
+        <bottom style="thin">
+          <color theme="0"/>
+        </bottom>
       </border>
     </dxf>
     <dxf>
@@ -798,132 +821,6 @@
     </dxf>
     <dxf>
       <fill>
-        <patternFill patternType="solid">
-          <fgColor auto="1"/>
-          <bgColor theme="7"/>
-        </patternFill>
-      </fill>
-      <border>
-        <bottom style="thin">
-          <color theme="0"/>
-        </bottom>
-      </border>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="0"/>
-        </patternFill>
-      </fill>
-      <border>
-        <bottom style="thin">
-          <color theme="0"/>
-        </bottom>
-        <vertical/>
-        <horizontal/>
-      </border>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="0" tint="-4.9989318521683403E-2"/>
-        </patternFill>
-      </fill>
-      <border>
-        <bottom style="thin">
-          <color theme="0"/>
-        </bottom>
-        <vertical/>
-        <horizontal/>
-      </border>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="9" tint="0.59996337778862885"/>
-        </patternFill>
-      </fill>
-      <border>
-        <left style="thin">
-          <color theme="9" tint="-0.24994659260841701"/>
-        </left>
-        <right style="thin">
-          <color theme="9" tint="-0.24994659260841701"/>
-        </right>
-        <bottom style="thin">
-          <color theme="9" tint="0.59996337778862885"/>
-        </bottom>
-        <vertical/>
-        <horizontal/>
-      </border>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="lightUp">
-          <fgColor theme="7"/>
-          <bgColor auto="1"/>
-        </patternFill>
-      </fill>
-      <border>
-        <bottom style="thin">
-          <color theme="0"/>
-        </bottom>
-      </border>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="lightUp">
-          <fgColor theme="7"/>
-          <bgColor theme="9" tint="0.59996337778862885"/>
-        </patternFill>
-      </fill>
-      <border>
-        <bottom style="thin">
-          <color theme="0"/>
-        </bottom>
-      </border>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="lightUp">
-          <fgColor theme="7"/>
-          <bgColor theme="7" tint="0.59996337778862885"/>
-        </patternFill>
-      </fill>
-      <border>
-        <bottom style="thin">
-          <color theme="0"/>
-        </bottom>
-      </border>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor auto="1"/>
-          <bgColor theme="9"/>
-        </patternFill>
-      </fill>
-      <border>
-        <bottom style="thin">
-          <color theme="0"/>
-        </bottom>
-      </border>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor auto="1"/>
-          <bgColor theme="7"/>
-        </patternFill>
-      </fill>
-      <border>
-        <bottom style="thin">
-          <color theme="0"/>
-        </bottom>
-      </border>
-    </dxf>
-    <dxf>
-      <fill>
         <patternFill>
           <bgColor theme="9" tint="0.59996337778862885"/>
         </patternFill>
@@ -953,10 +850,6 @@
     </ext>
   </extLst>
 </styleSheet>
-</file>
-
-<file path=xl/persons/person.xml><?xml version="1.0" encoding="utf-8"?>
-<personList xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main"/>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -1192,27 +1085,27 @@
   </sheetPr>
   <dimension ref="B1:BO39"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" zoomScale="34" zoomScaleNormal="100" zoomScaleSheetLayoutView="80" workbookViewId="0">
-      <selection activeCell="DD1" sqref="DD1"/>
+    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A12" zoomScale="75" zoomScaleNormal="100" zoomScaleSheetLayoutView="80" workbookViewId="0">
+      <selection activeCell="G33" sqref="G33"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="2.77734375" defaultRowHeight="30" customHeight="1" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="2.83203125" defaultRowHeight="30" customHeight="1" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="2.6640625" customWidth="1"/>
     <col min="2" max="2" width="26.33203125" style="2" customWidth="1"/>
-    <col min="3" max="3" width="11.44140625" style="1" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="10.21875" style="1" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="7.88671875" style="1" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="10.21875" style="1" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="15.5546875" style="4" bestFit="1" customWidth="1"/>
-    <col min="8" max="16" width="3.88671875" style="1" bestFit="1" customWidth="1"/>
-    <col min="17" max="27" width="5.44140625" style="1" bestFit="1" customWidth="1"/>
-    <col min="28" max="41" width="5.44140625" bestFit="1" customWidth="1"/>
-    <col min="42" max="42" width="2.77734375" customWidth="1"/>
-    <col min="43" max="67" width="5.44140625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="11.5" style="1" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="10.1640625" style="1" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="7.83203125" style="1" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="10.1640625" style="1" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="15.5" style="4" bestFit="1" customWidth="1"/>
+    <col min="8" max="16" width="3.83203125" style="1" bestFit="1" customWidth="1"/>
+    <col min="17" max="27" width="5.5" style="1" bestFit="1" customWidth="1"/>
+    <col min="28" max="41" width="5.5" bestFit="1" customWidth="1"/>
+    <col min="42" max="42" width="2.83203125" customWidth="1"/>
+    <col min="43" max="67" width="5.5" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="2:67" ht="60" customHeight="1" thickBot="1" x14ac:dyDescent="1.05">
+    <row r="1" spans="2:67" ht="60" customHeight="1" thickBot="1" x14ac:dyDescent="0.85">
       <c r="B1" s="14" t="s">
         <v>49</v>
       </c>
@@ -1222,14 +1115,14 @@
       <c r="F1" s="13"/>
       <c r="G1" s="13"/>
     </row>
-    <row r="2" spans="2:67" ht="21" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B2" s="34" t="s">
+    <row r="2" spans="2:67" ht="21" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="B2" s="25" t="s">
         <v>39</v>
       </c>
-      <c r="C2" s="34"/>
-      <c r="D2" s="34"/>
-      <c r="E2" s="34"/>
-      <c r="F2" s="34"/>
+      <c r="C2" s="25"/>
+      <c r="D2" s="25"/>
+      <c r="E2" s="25"/>
+      <c r="F2" s="25"/>
       <c r="G2" s="5" t="s">
         <v>31</v>
       </c>
@@ -1237,37 +1130,37 @@
         <v>1</v>
       </c>
       <c r="J2" s="16"/>
-      <c r="K2" s="27" t="s">
+      <c r="K2" s="31" t="s">
         <v>38</v>
       </c>
-      <c r="L2" s="28"/>
-      <c r="M2" s="28"/>
-      <c r="N2" s="28"/>
-      <c r="O2" s="29"/>
+      <c r="L2" s="32"/>
+      <c r="M2" s="32"/>
+      <c r="N2" s="32"/>
+      <c r="O2" s="33"/>
       <c r="P2" s="17"/>
-      <c r="Q2" s="27" t="s">
+      <c r="Q2" s="31" t="s">
         <v>37</v>
       </c>
-      <c r="R2" s="30"/>
-      <c r="S2" s="30"/>
-      <c r="T2" s="29"/>
+      <c r="R2" s="34"/>
+      <c r="S2" s="34"/>
+      <c r="T2" s="33"/>
       <c r="U2" s="18"/>
-      <c r="V2" s="31" t="s">
+      <c r="V2" s="35" t="s">
         <v>28</v>
       </c>
-      <c r="W2" s="32"/>
-      <c r="X2" s="32"/>
-      <c r="Y2" s="33"/>
+      <c r="W2" s="36"/>
+      <c r="X2" s="36"/>
+      <c r="Y2" s="37"/>
       <c r="Z2" s="19"/>
-      <c r="AA2" s="31" t="s">
+      <c r="AA2" s="35" t="s">
         <v>29</v>
       </c>
-      <c r="AB2" s="32"/>
-      <c r="AC2" s="32"/>
-      <c r="AD2" s="32"/>
-      <c r="AE2" s="32"/>
-      <c r="AF2" s="32"/>
-      <c r="AG2" s="33"/>
+      <c r="AB2" s="36"/>
+      <c r="AC2" s="36"/>
+      <c r="AD2" s="36"/>
+      <c r="AE2" s="36"/>
+      <c r="AF2" s="36"/>
+      <c r="AG2" s="37"/>
       <c r="AH2" s="20"/>
       <c r="AI2" s="22" t="s">
         <v>30</v>
@@ -1280,23 +1173,23 @@
       <c r="AO2" s="23"/>
       <c r="AP2" s="23"/>
     </row>
-    <row r="3" spans="2:67" s="12" customFormat="1" ht="39.9" customHeight="1" thickTop="1" x14ac:dyDescent="0.3">
-      <c r="B3" s="35" t="s">
-        <v>1</v>
-      </c>
-      <c r="C3" s="37" t="s">
+    <row r="3" spans="2:67" s="12" customFormat="1" ht="40" customHeight="1" thickTop="1" x14ac:dyDescent="0.2">
+      <c r="B3" s="26" t="s">
+        <v>1</v>
+      </c>
+      <c r="C3" s="28" t="s">
         <v>32</v>
       </c>
-      <c r="D3" s="37" t="s">
+      <c r="D3" s="28" t="s">
         <v>33</v>
       </c>
-      <c r="E3" s="37" t="s">
+      <c r="E3" s="28" t="s">
         <v>34</v>
       </c>
-      <c r="F3" s="37" t="s">
+      <c r="F3" s="28" t="s">
         <v>35</v>
       </c>
-      <c r="G3" s="25" t="s">
+      <c r="G3" s="30" t="s">
         <v>36</v>
       </c>
       <c r="H3" s="21" t="s">
@@ -1322,13 +1215,13 @@
       <c r="Z3" s="11"/>
       <c r="AA3" s="11"/>
     </row>
-    <row r="4" spans="2:67" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B4" s="36"/>
-      <c r="C4" s="26"/>
-      <c r="D4" s="26"/>
-      <c r="E4" s="26"/>
-      <c r="F4" s="26"/>
-      <c r="G4" s="26"/>
+    <row r="4" spans="2:67" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="B4" s="27"/>
+      <c r="C4" s="29"/>
+      <c r="D4" s="29"/>
+      <c r="E4" s="29"/>
+      <c r="F4" s="29"/>
+      <c r="G4" s="29"/>
       <c r="H4" s="3">
         <v>1</v>
       </c>
@@ -1510,7 +1403,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="5" spans="2:67" ht="30" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="5" spans="2:67" ht="30" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="B5" s="6" t="s">
         <v>2</v>
       </c>
@@ -1535,7 +1428,7 @@
       <c r="K5" s="24"/>
       <c r="L5" s="24"/>
     </row>
-    <row r="6" spans="2:67" ht="30" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="6" spans="2:67" ht="30" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="B6" s="6" t="s">
         <v>3</v>
       </c>
@@ -1557,7 +1450,7 @@
       <c r="H6" s="18"/>
       <c r="L6" s="17"/>
     </row>
-    <row r="7" spans="2:67" ht="30" customHeight="1" thickTop="1" x14ac:dyDescent="0.35">
+    <row r="7" spans="2:67" ht="30" customHeight="1" thickTop="1" x14ac:dyDescent="0.2">
       <c r="B7" s="6" t="s">
         <v>4</v>
       </c>
@@ -1577,7 +1470,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="8" spans="2:67" ht="30" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="8" spans="2:67" ht="30" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B8" s="6" t="s">
         <v>5</v>
       </c>
@@ -1597,7 +1490,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="9" spans="2:67" ht="30" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="9" spans="2:67" ht="30" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B9" s="6" t="s">
         <v>6</v>
       </c>
@@ -1617,7 +1510,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="10" spans="2:67" ht="30" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="10" spans="2:67" ht="30" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B10" s="6" t="s">
         <v>7</v>
       </c>
@@ -1637,7 +1530,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="11" spans="2:67" ht="30" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="11" spans="2:67" ht="30" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B11" s="6" t="s">
         <v>8</v>
       </c>
@@ -1657,7 +1550,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="12" spans="2:67" ht="30" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="12" spans="2:67" ht="30" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B12" s="6" t="s">
         <v>9</v>
       </c>
@@ -1677,7 +1570,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="13" spans="2:67" ht="30" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="13" spans="2:67" ht="30" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B13" s="6" t="s">
         <v>10</v>
       </c>
@@ -1697,7 +1590,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="14" spans="2:67" ht="30" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="14" spans="2:67" ht="30" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B14" s="6" t="s">
         <v>11</v>
       </c>
@@ -1717,7 +1610,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="15" spans="2:67" ht="30" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="15" spans="2:67" ht="30" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B15" s="6" t="s">
         <v>12</v>
       </c>
@@ -1737,7 +1630,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="16" spans="2:67" ht="30" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="16" spans="2:67" ht="30" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B16" s="6" t="s">
         <v>13</v>
       </c>
@@ -1757,7 +1650,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="17" spans="2:7" ht="30" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="17" spans="2:18" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="B17" s="6" t="s">
         <v>14</v>
       </c>
@@ -1774,10 +1667,10 @@
         <v>5</v>
       </c>
       <c r="G17" s="8">
-        <v>0.9</v>
-      </c>
-    </row>
-    <row r="18" spans="2:7" ht="30" customHeight="1" x14ac:dyDescent="0.35">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="18" spans="2:18" ht="30" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="B18" s="6" t="s">
         <v>15</v>
       </c>
@@ -1794,10 +1687,11 @@
         <v>6</v>
       </c>
       <c r="G18" s="8">
-        <v>0.9</v>
-      </c>
-    </row>
-    <row r="19" spans="2:7" ht="30" customHeight="1" x14ac:dyDescent="0.35">
+        <v>1</v>
+      </c>
+      <c r="R18" s="18"/>
+    </row>
+    <row r="19" spans="2:18" ht="30" customHeight="1" thickTop="1" x14ac:dyDescent="0.2">
       <c r="B19" s="6" t="s">
         <v>16</v>
       </c>
@@ -1814,10 +1708,10 @@
         <v>6</v>
       </c>
       <c r="G19" s="8">
-        <v>0.5</v>
-      </c>
-    </row>
-    <row r="20" spans="2:7" ht="30" customHeight="1" x14ac:dyDescent="0.35">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="20" spans="2:18" ht="30" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B20" s="6" t="s">
         <v>17</v>
       </c>
@@ -1827,13 +1721,17 @@
       <c r="D20" s="7">
         <v>8</v>
       </c>
-      <c r="E20" s="7"/>
-      <c r="F20" s="7"/>
-      <c r="G20" s="8">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="21" spans="2:7" ht="30" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="E20" s="7">
+        <v>8</v>
+      </c>
+      <c r="F20" s="7">
+        <v>8</v>
+      </c>
+      <c r="G20" s="38">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="21" spans="2:18" ht="30" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B21" s="6" t="s">
         <v>18</v>
       </c>
@@ -1843,13 +1741,17 @@
       <c r="D21" s="7">
         <v>14</v>
       </c>
-      <c r="E21" s="7"/>
-      <c r="F21" s="7"/>
+      <c r="E21" s="7">
+        <v>10</v>
+      </c>
+      <c r="F21" s="7">
+        <v>16</v>
+      </c>
       <c r="G21" s="8">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="22" spans="2:7" ht="30" customHeight="1" x14ac:dyDescent="0.35">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="22" spans="2:18" ht="30" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B22" s="6" t="s">
         <v>19</v>
       </c>
@@ -1859,13 +1761,17 @@
       <c r="D22" s="7">
         <v>15</v>
       </c>
-      <c r="E22" s="7"/>
-      <c r="F22" s="7"/>
+      <c r="E22" s="7">
+        <v>18</v>
+      </c>
+      <c r="F22" s="7">
+        <v>15</v>
+      </c>
       <c r="G22" s="8">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="23" spans="2:7" ht="30" customHeight="1" x14ac:dyDescent="0.35">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="23" spans="2:18" ht="30" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B23" s="6" t="s">
         <v>20</v>
       </c>
@@ -1875,13 +1781,17 @@
       <c r="D23" s="7">
         <v>16</v>
       </c>
-      <c r="E23" s="7"/>
-      <c r="F23" s="7"/>
+      <c r="E23" s="7">
+        <v>16</v>
+      </c>
+      <c r="F23" s="7">
+        <v>18</v>
+      </c>
       <c r="G23" s="8">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="24" spans="2:7" ht="30" customHeight="1" x14ac:dyDescent="0.35">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="24" spans="2:18" ht="30" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B24" s="6" t="s">
         <v>21</v>
       </c>
@@ -1891,13 +1801,17 @@
       <c r="D24" s="7">
         <v>17</v>
       </c>
-      <c r="E24" s="7"/>
-      <c r="F24" s="7"/>
+      <c r="E24" s="7">
+        <v>17</v>
+      </c>
+      <c r="F24" s="7">
+        <v>17</v>
+      </c>
       <c r="G24" s="8">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="25" spans="2:7" ht="30" customHeight="1" x14ac:dyDescent="0.35">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="25" spans="2:18" ht="30" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B25" s="6" t="s">
         <v>22</v>
       </c>
@@ -1907,13 +1821,17 @@
       <c r="D25" s="7">
         <v>17</v>
       </c>
-      <c r="E25" s="7"/>
-      <c r="F25" s="7"/>
+      <c r="E25" s="7">
+        <v>18</v>
+      </c>
+      <c r="F25" s="7">
+        <v>17</v>
+      </c>
       <c r="G25" s="8">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="26" spans="2:7" ht="30" customHeight="1" x14ac:dyDescent="0.35">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="26" spans="2:18" ht="30" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B26" s="6" t="s">
         <v>23</v>
       </c>
@@ -1923,13 +1841,17 @@
       <c r="D26" s="7">
         <v>18</v>
       </c>
-      <c r="E26" s="7"/>
-      <c r="F26" s="7"/>
+      <c r="E26" s="7">
+        <v>20</v>
+      </c>
+      <c r="F26" s="7">
+        <v>18</v>
+      </c>
       <c r="G26" s="8">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="27" spans="2:7" ht="30" customHeight="1" x14ac:dyDescent="0.35">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="27" spans="2:18" ht="30" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B27" s="6" t="s">
         <v>24</v>
       </c>
@@ -1939,13 +1861,17 @@
       <c r="D27" s="7">
         <v>19</v>
       </c>
-      <c r="E27" s="7"/>
-      <c r="F27" s="7"/>
+      <c r="E27" s="7">
+        <v>20</v>
+      </c>
+      <c r="F27" s="7">
+        <v>20</v>
+      </c>
       <c r="G27" s="8">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="28" spans="2:7" ht="30" customHeight="1" x14ac:dyDescent="0.35">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="28" spans="2:18" ht="30" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B28" s="6" t="s">
         <v>25</v>
       </c>
@@ -1955,13 +1881,17 @@
       <c r="D28" s="7">
         <v>20</v>
       </c>
-      <c r="E28" s="7"/>
-      <c r="F28" s="7"/>
+      <c r="E28" s="7">
+        <v>21</v>
+      </c>
+      <c r="F28" s="7">
+        <v>20</v>
+      </c>
       <c r="G28" s="8">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="29" spans="2:7" ht="30" customHeight="1" x14ac:dyDescent="0.35">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="29" spans="2:18" ht="30" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B29" s="6" t="s">
         <v>26</v>
       </c>
@@ -1971,13 +1901,17 @@
       <c r="D29" s="7">
         <v>20</v>
       </c>
-      <c r="E29" s="7"/>
-      <c r="F29" s="7"/>
+      <c r="E29" s="7">
+        <v>22</v>
+      </c>
+      <c r="F29" s="7">
+        <v>20</v>
+      </c>
       <c r="G29" s="8">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="30" spans="2:7" ht="30" customHeight="1" x14ac:dyDescent="0.35">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="30" spans="2:18" ht="30" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B30" s="6" t="s">
         <v>27</v>
       </c>
@@ -1987,13 +1921,17 @@
       <c r="D30" s="7">
         <v>21</v>
       </c>
-      <c r="E30" s="7"/>
-      <c r="F30" s="7"/>
+      <c r="E30" s="7">
+        <v>21</v>
+      </c>
+      <c r="F30" s="7">
+        <v>25</v>
+      </c>
       <c r="G30" s="8">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="31" spans="2:7" ht="30" customHeight="1" x14ac:dyDescent="0.35">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="31" spans="2:18" ht="30" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B31" s="6" t="s">
         <v>40</v>
       </c>
@@ -2003,13 +1941,17 @@
       <c r="D31" s="7">
         <v>21</v>
       </c>
-      <c r="E31" s="7"/>
-      <c r="F31" s="7"/>
+      <c r="E31" s="7">
+        <v>21</v>
+      </c>
+      <c r="F31" s="7">
+        <v>25</v>
+      </c>
       <c r="G31" s="8">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="32" spans="2:7" ht="30" customHeight="1" x14ac:dyDescent="0.35">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="32" spans="2:18" ht="30" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B32" s="6" t="s">
         <v>41</v>
       </c>
@@ -2019,13 +1961,17 @@
       <c r="D32" s="7">
         <v>23</v>
       </c>
-      <c r="E32" s="7"/>
-      <c r="F32" s="7"/>
+      <c r="E32" s="7">
+        <v>22</v>
+      </c>
+      <c r="F32" s="7">
+        <v>27</v>
+      </c>
       <c r="G32" s="8">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="33" spans="2:7" ht="30" customHeight="1" x14ac:dyDescent="0.35">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="33" spans="2:7" ht="30" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B33" s="6" t="s">
         <v>42</v>
       </c>
@@ -2035,13 +1981,17 @@
       <c r="D33" s="7">
         <v>24</v>
       </c>
-      <c r="E33" s="7"/>
-      <c r="F33" s="7"/>
+      <c r="E33" s="7">
+        <v>24</v>
+      </c>
+      <c r="F33" s="7">
+        <v>26</v>
+      </c>
       <c r="G33" s="8">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="34" spans="2:7" ht="30" customHeight="1" x14ac:dyDescent="0.35">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="34" spans="2:7" ht="30" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B34" s="6" t="s">
         <v>43</v>
       </c>
@@ -2053,7 +2003,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="35" spans="2:7" ht="30" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="35" spans="2:7" ht="30" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B35" s="6" t="s">
         <v>44</v>
       </c>
@@ -2065,7 +2015,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="36" spans="2:7" ht="30" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="36" spans="2:7" ht="30" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B36" s="6" t="s">
         <v>45</v>
       </c>
@@ -2077,7 +2027,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="37" spans="2:7" ht="30" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="37" spans="2:7" ht="30" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B37" s="6" t="s">
         <v>46</v>
       </c>
@@ -2089,7 +2039,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="38" spans="2:7" ht="30" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="38" spans="2:7" ht="30" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B38" s="6" t="s">
         <v>47</v>
       </c>
@@ -2101,7 +2051,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="39" spans="2:7" ht="30" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="39" spans="2:7" ht="30" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B39" s="6" t="s">
         <v>48</v>
       </c>
@@ -2115,46 +2065,46 @@
     </row>
   </sheetData>
   <mergeCells count="11">
+    <mergeCell ref="G3:G4"/>
+    <mergeCell ref="K2:O2"/>
+    <mergeCell ref="Q2:T2"/>
+    <mergeCell ref="V2:Y2"/>
+    <mergeCell ref="AA2:AG2"/>
     <mergeCell ref="B2:F2"/>
     <mergeCell ref="B3:B4"/>
     <mergeCell ref="C3:C4"/>
     <mergeCell ref="D3:D4"/>
     <mergeCell ref="E3:E4"/>
     <mergeCell ref="F3:F4"/>
-    <mergeCell ref="G3:G4"/>
-    <mergeCell ref="K2:O2"/>
-    <mergeCell ref="Q2:T2"/>
-    <mergeCell ref="V2:Y2"/>
-    <mergeCell ref="AA2:AG2"/>
   </mergeCells>
   <conditionalFormatting sqref="H4:BO4">
-    <cfRule type="expression" dxfId="16" priority="8">
+    <cfRule type="expression" dxfId="8" priority="8">
       <formula>H$4=period_selected</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="I5:BO5 I6:K6 M6:BO6 H7:BO39">
-    <cfRule type="expression" dxfId="15" priority="1">
+    <cfRule type="expression" dxfId="7" priority="3">
+      <formula>PercentCompleteBeyond</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="6" priority="4">
+      <formula>Actual</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="5" priority="5">
+      <formula>ActualBeyond</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="4" priority="6">
+      <formula>Plan</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="3" priority="7">
+      <formula>H$4=period_selected</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="2" priority="1">
       <formula>PercentComplete</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="14" priority="3">
-      <formula>PercentCompleteBeyond</formula>
-    </cfRule>
-    <cfRule type="expression" dxfId="13" priority="4">
-      <formula>Actual</formula>
-    </cfRule>
-    <cfRule type="expression" dxfId="12" priority="5">
-      <formula>ActualBeyond</formula>
-    </cfRule>
-    <cfRule type="expression" dxfId="11" priority="6">
-      <formula>Plan</formula>
-    </cfRule>
-    <cfRule type="expression" dxfId="10" priority="7">
-      <formula>H$4=period_selected</formula>
-    </cfRule>
-    <cfRule type="expression" dxfId="9" priority="11">
+    <cfRule type="expression" dxfId="1" priority="11">
       <formula>MOD(COLUMN(),2)</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="8" priority="12">
+    <cfRule type="expression" dxfId="0" priority="12">
       <formula>MOD(COLUMN(),2)=0</formula>
     </cfRule>
   </conditionalFormatting>
@@ -2190,4 +2140,10 @@
     </ext>
   </extLst>
 </worksheet>
+</file>
+
+<file path=docMetadata/LabelInfo.xml><?xml version="1.0" encoding="utf-8"?>
+<clbl:labelList xmlns:clbl="http://schemas.microsoft.com/office/2020/mipLabelMetadata">
+  <clbl:label id="{c9f92db8-2851-4df9-9d12-fab52f5b1415}" enabled="1" method="Standard" siteId="{5a7cc8ab-a4dc-4f9b-bf60-66714049ad62}" contentBits="0" removed="0"/>
+</clbl:labelList>
 </file>
</xml_diff>